<commit_message>
fix shope update problem
</commit_message>
<xml_diff>
--- a/src/electron/crawler/config/小米粒夏日.xlsx
+++ b/src/electron/crawler/config/小米粒夏日.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27932"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\outsider\github\GF_playwright\src\electron\crawler\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C72B36BE-D31B-48ED-8730-F4312E516D08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29038997-0AA8-44DF-AFB5-83E37B8B4B9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3675" yWindow="3675" windowWidth="21600" windowHeight="11393" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>流水號</t>
   </si>
@@ -28,113 +28,146 @@
     <t>content</t>
   </si>
   <si>
-    <t>【cimYL065】實拍氣質小姊姊的圓領麻花針織衫240313</t>
-  </si>
-  <si>
-    <t>胸圍86 肩寬39 袖長21 衣長54
-誤差1-3公分為正常，以實物為準。</t>
-  </si>
-  <si>
-    <t>【cimYL083】實拍早春温柔顯白簡約針織吊帶背心240313</t>
-  </si>
-  <si>
-    <t>胸圍68 肩寬 27 袖長/ 衣長42
-誤差1-3公分為正常，以實物為準。</t>
-  </si>
-  <si>
-    <t>【cimYL093】實拍早春温柔百搭短袖針織衫240313</t>
-  </si>
-  <si>
-    <t>胸圍80 肩寬31 袖長22 衣長49
-誤差1-3公分為正常，以實物為準。</t>
-  </si>
-  <si>
-    <t>【cimYL217】實拍早春簡約休閒連帽長袖針織衫240313</t>
-  </si>
-  <si>
-    <t>胸圍92 肩寬39 袖長58 衣長56
-誤差1-3公分為正常，以實物為準。</t>
-  </si>
-  <si>
-    <t>【cim2380】實拍早春法式優雅氣質蝴蝶結仙氣温柔長袖襯衫240313</t>
-  </si>
-  <si>
-    <t>M 胸圍92 肩寬36 袖長61 衣長57
-L 胸圍94 肩寬38 袖長63 衣長59
-誤差1-3公分為正常，以實物為準。</t>
-  </si>
-  <si>
-    <t>【cim2381】實拍春日鬆弛感中性復古條紋襯衫240313</t>
-  </si>
-  <si>
-    <t>M 胸圍94 肩寬44 袖長54 衣長68
-L 胸圍96 肩寬46 袖長56 衣長70
-誤差1-3公分為正常，以實物為準。</t>
-  </si>
-  <si>
-    <t>【cim2383】實拍小眾日系款~復古純色慵懶上衣240313</t>
-  </si>
-  <si>
-    <t>M 胸圍100 肩寬75 袖長/ 衣長49
-L 胸圍102 肩寬77 袖長/ 衣長51
-誤差1-3公分為正常，以實物為準。</t>
-  </si>
-  <si>
-    <t>【cimYL907】實拍復古方領吊帶顯瘦大擺針織裙240313</t>
-  </si>
-  <si>
-    <t>腰圍68-80 臀圍/ 裙長105
-誤差1-3公分為正常，以實物為準。</t>
-  </si>
-  <si>
-    <t>【cim2385】實拍混搭微透刺繡鈎花泡泡袖連衣裙240313</t>
-  </si>
-  <si>
-    <t>M 胸圍/ 腰圍85/78 肩寬28 袖長20 裙長106
-L 胸圍/ 腰圍84/80 肩寬30 袖長21 裙長108
-誤差1-3公分為正常，以實物為準。</t>
-  </si>
-  <si>
-    <t>【cimYL215】實拍法式復古風假兩件針織吊帶裙240313</t>
-  </si>
-  <si>
-    <t>胸圍64. 裙長115
-誤差1-3公分為正常，以實物為準。</t>
-  </si>
-  <si>
-    <t>【cimYL1165】實拍早春U領短袖軟糯薄款針織衫240313</t>
-  </si>
-  <si>
-    <t>胸圍66 肩寬34 袖長28 衣長60
-誤差1-3公分為正常，以實物為準。</t>
-  </si>
-  <si>
-    <t>【cimYL052】實拍質感温柔金扣短款針織衫240313</t>
-  </si>
-  <si>
-    <t>胸圍90 肩寬39 袖長 60 衣長51
-誤差1-3公分為正常，以實物為準。</t>
-  </si>
-  <si>
-    <t>【cimYL018】實拍質感圓領針織背心240313</t>
-  </si>
-  <si>
-    <t>胸圍68 肩寬30 袖長 / 衣長51
-誤差1-3公分為正常，以實物為準。</t>
-  </si>
-  <si>
-    <t>【cimYL020】實拍温柔氣質細坑條針織衫240313</t>
-  </si>
-  <si>
-    <t>胸圍 84 肩寬37 袖長26 衣長58
-誤差1-3公分為正常，以實物為準。</t>
+    <t>【Y96031】實拍S~XL韓版高腰顯瘦白色直筒九分牛仔褲240925</t>
+  </si>
+  <si>
+    <t>S：腰圍 64，臀圍 94，大腿圍 60，褲腳圍 58，褲長 95
+M：腰圍 68，臀圍 98，大腿圍 62，褲腳圍 60，褲長 96
+L：腰圍 72，臀圍 102，大腿圍 64，褲腳圍 62，褲長 97
+XL：腰圍 76，臀圍 106，大腿圍 66，褲腳圍 64，褲長 98
+手工平鋪測量，誤差允許在1~3cm左右，具體以實物為準。</t>
+  </si>
+  <si>
+    <t>【YG9631】實拍秋季休閒慵懶褶皺假兩件針織衫(6%羊毛)240925</t>
+  </si>
+  <si>
+    <t>肩寬 38，袖長 63，胸圍 76，下擺圍 74，衣長 58
+手工平鋪測量，誤差允許在1~3cm左右，具體以實物為準。</t>
+  </si>
+  <si>
+    <t>【Y9789】實拍法式復古高腰百褶A字裙240925</t>
+  </si>
+  <si>
+    <t>M：腰圍 60，臀圍 110，下擺圍 226，袖長 92
+L：腰圍 64，臀圍 114，下擺圍 230，袖長 93
+手工平鋪測量，誤差允許在1~3cm左右，具體以實物為準</t>
+  </si>
+  <si>
+    <t>【Y82136】實拍韓國寬鬆不規則側開叉斜扣純棉襯衫240925</t>
+  </si>
+  <si>
+    <t>M：肩寬 48，袖長 59.5，胸圍 122，下擺圍 130，衣長 71/75
+L：肩寬 49，袖長 60.5，胸圍 126，下擺圍 134，衣長 72/76
+手工平鋪測量，誤差允許在1~3cm左右，具體以實物為準</t>
+  </si>
+  <si>
+    <t>【Y9790】實拍韓國設計款休閒質感衞褲240925</t>
+  </si>
+  <si>
+    <t>M：腰圍 66，臀圍 124，大腿圍 76，褲腳圍 58，褲長 102
+L：腰圍 70，臀圍 128，大腿圍 78，褲腳圍 60，褲長 103
+手工平鋪測量，誤差允許在1~3cm左右，具體以實物為準</t>
+  </si>
+  <si>
+    <t>【YA12】實拍軟軟舒服的針織外套+針織背心 套裝240925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F（背心）：胸圍 72，下擺圍 78，衣長 48
+F（外套）：肩寬 60，袖長 46，胸圍 110，下擺圍 110，衣長 76
+手工平鋪測量，誤差允許在1~3cm左右，具體以實物為準。
+</t>
+  </si>
+  <si>
+    <t>【YP661】實拍慵懶垂感高腰針織闊腿褲240925</t>
+  </si>
+  <si>
+    <t xml:space="preserve">腰圍 61，臀圍 120，大腿圍 88，褲腳圍 134，褲長 94
+手工平鋪測量，誤差允許在1~3cm左右，具體以實物為準。
+</t>
+  </si>
+  <si>
+    <t>【YG9662】實拍休閒撞色假兩件T恤針織衫240925</t>
+  </si>
+  <si>
+    <t>肩寬 36，袖長 61，胸圍 76，下擺圍 76，衣長 55
+手工平鋪測量，誤差允許在1~3cm左右，具體以實物為準。</t>
+  </si>
+  <si>
+    <t>【YG5162】實拍氣質百搭方領坑條長袖針織衫240925</t>
+  </si>
+  <si>
+    <t>肩寬 35，袖長 58，胸圍 66，下擺圍 66，衣長 55
+手工平鋪測量，誤差允許在1~3cm左右，具體以實物為準。</t>
+  </si>
+  <si>
+    <t>【YA8】實拍韓系簡約V領寬鬆針織外套240925</t>
+  </si>
+  <si>
+    <t>袖長 67，胸圍 100，下擺圍 86，衣長 52
+手工平鋪測量，誤差允許在1~3cm左右，具體以實物為準。</t>
+  </si>
+  <si>
+    <t>【Y68106】實拍S~XL高腰顯瘦直筒牛仔褲240925</t>
+  </si>
+  <si>
+    <t>S：腰圍 66，臀圍 96，大腿圍 60，褲腳圍 50，褲長 103
+M：腰圍 70，臀圍 100，大腿圍 62，褲腳圍 52，褲長 104
+L：腰圍 74，臀圍 104，大腿圍 64，褲腳圍 54，褲長 105
+XL：腰圍 78，臀圍 108，大腿圍 66，褲腳圍 56，褲長 106
+手工平鋪測量，誤差允許在1~3cm左右，具體以實物為準。</t>
+  </si>
+  <si>
+    <t>【YH9607】實拍S~XL復古高腰直筒牛仔褲240925</t>
+  </si>
+  <si>
+    <t>S：腰圍 64，臀圍 92，大腿圍 60，褲腳圍 48，褲長 91
+M：腰圍 68，臀圍 96，大腿圍 62，褲腳圍 50，褲長 92
+L：腰圍 72，臀圍 100，大腿圍 64，褲腳圍 52，褲長 93
+XL：腰圍 76，臀圍 104，大腿圍 66，褲腳圍 54，褲長 94
+手工平鋪測量，誤差允許在1~3cm左右，具體以實物為準。</t>
+  </si>
+  <si>
+    <t>【YP332】實拍韓版半高領軟糯針織T恤洋裝240925</t>
+  </si>
+  <si>
+    <t>肩寬 39，袖長 22，胸圍 94，下擺圍 104，衣長 124
+手工平鋪測量，誤差允許在1~3cm左右，具體以實物為準。</t>
+  </si>
+  <si>
+    <t>【YG9833】實拍半拉鍊假兩件針織T恤(6%羊毛)240925</t>
+  </si>
+  <si>
+    <t>肩寬 38，袖長 63，胸圍 70，下擺圍 68，衣長 50/55
+手工平鋪測量，誤差允許在1~3cm左右，具體以實物為準。</t>
+  </si>
+  <si>
+    <t>【YG736】實拍簡約設計感修身長袖針織T恤(6%羊毛)240925</t>
+  </si>
+  <si>
+    <t>肩寬 33，袖長 62，胸圍 72，下擺圍 74，衣長 56
+手工平鋪測量，誤差允許在1~3cm左右，具體以實物為準。</t>
+  </si>
+  <si>
+    <t>【YA13】實拍氣質針織外套＋背心兩件套240925</t>
+  </si>
+  <si>
+    <t>F（背心）：胸圍 68，下擺圍 66，衣長 49
+F（外套）：肩寬 57，袖長 54，胸圍 116，下擺圍 114，衣長 58
+手工平鋪測量，誤差允許在1~3cm左右，具體以實物為準。</t>
+  </si>
+  <si>
+    <t>【YXXT325】實拍簡約粗針針織背心(羊毛25)240925</t>
+  </si>
+  <si>
+    <t>肩寬 47，胸圍 100，下擺圍 90，衣長 54
+手工平鋪測量，誤差允許在1~3cm左右，具體以實物為準。</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -159,12 +192,6 @@
       <color theme="1"/>
       <name val="PingFang TC"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -186,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -212,15 +239,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -501,7 +522,7 @@
   <dimension ref="A1:B36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B15"/>
+      <selection activeCell="A2" sqref="A2:B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75"/>
@@ -518,7 +539,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="77.650000000000006">
+    <row r="2" spans="1:2" ht="205.15">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -534,7 +555,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="77.650000000000006">
+    <row r="4" spans="1:2" ht="128.65">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -542,7 +563,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="77.650000000000006">
+    <row r="5" spans="1:2" ht="115.9">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
@@ -550,7 +571,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="90.4">
+    <row r="6" spans="1:2" ht="115.9">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
@@ -558,15 +579,15 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="90.4">
+    <row r="7" spans="1:2" ht="63.75">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="8" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="90.4">
+    <row r="8" spans="1:2" ht="103.15">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
@@ -582,15 +603,15 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="63.75">
+    <row r="10" spans="1:2" ht="64.900000000000006">
       <c r="A10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="64.900000000000006">
+    <row r="11" spans="1:2" ht="77.650000000000006">
       <c r="A11" s="1" t="s">
         <v>20</v>
       </c>
@@ -598,7 +619,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="77.650000000000006">
+    <row r="12" spans="1:2" ht="192.4">
       <c r="A12" s="1" t="s">
         <v>22</v>
       </c>
@@ -606,7 +627,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="77.650000000000006">
+    <row r="13" spans="1:2" ht="192.4">
       <c r="A13" s="1" t="s">
         <v>24</v>
       </c>
@@ -630,17 +651,29 @@
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="9"/>
-      <c r="B16" s="10"/>
-    </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="7"/>
-      <c r="B17" s="8"/>
-    </row>
-    <row r="18" spans="1:2">
-      <c r="A18" s="7"/>
-      <c r="B18" s="8"/>
+    <row r="16" spans="1:2" ht="64.900000000000006">
+      <c r="A16" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" ht="51">
+      <c r="A17" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" ht="64.900000000000006">
+      <c r="A18" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="7"/>

</xml_diff>